<commit_message>
Se agrega cambio a la tarea y un nuevo archivo de muestra
</commit_message>
<xml_diff>
--- a/ejemplos_clase/planning/Test_Case_Template TAREA correcciones.xlsx
+++ b/ejemplos_clase/planning/Test_Case_Template TAREA correcciones.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\repo\intro_automation\ejemplos_clase\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD3D463-4EC6-4058-802A-8CC4F2B0E02D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92FDCF8A-84E2-4E16-A074-8E73DED7C6EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2055" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>01</t>
-  </si>
-  <si>
-    <t>Login exitoso de la pagina</t>
   </si>
   <si>
     <t>El usuario debe estar registrado en la pagina "https://evening-bastion-49392.herokuapp.com/", debe contar con un usuario y password, ademas de usar su navegador de preferencia actualizado a la version mas reciente, para asi evitar problemas de compatibilidad</t>
@@ -409,6 +406,9 @@
   <si>
     <t>document.querySelectorAll('#songs a')[0].innerText</t>
   </si>
+  <si>
+    <t>Login exitoso de la pagina "Songs by Sinatra"</t>
+  </si>
 </sst>
 </file>
 
@@ -530,14 +530,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -855,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:E12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15"/>
@@ -891,10 +891,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>5</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -930,19 +930,19 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -952,16 +952,16 @@
         <v>1</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>41</v>
+      <c r="E7" s="24" t="s">
+        <v>40</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -971,15 +971,15 @@
         <v>2</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="22"/>
+      <c r="E8" s="24"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
@@ -988,15 +988,15 @@
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="D9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="22"/>
+      <c r="E9" s="24"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
@@ -1005,15 +1005,15 @@
         <v>4</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="D10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="22"/>
+      <c r="E10" s="24"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
@@ -1022,15 +1022,15 @@
         <v>5</v>
       </c>
       <c r="B11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>24</v>
-      </c>
       <c r="D11" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="22"/>
+        <v>15</v>
+      </c>
+      <c r="E11" s="24"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
@@ -1039,15 +1039,15 @@
         <v>6</v>
       </c>
       <c r="B12" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="D12" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="22"/>
+        <v>18</v>
+      </c>
+      <c r="E12" s="24"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
@@ -9994,30 +9994,30 @@
     </row>
     <row r="2" spans="1:5" ht="120">
       <c r="A2" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="C2" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="17" customFormat="1" ht="345">
@@ -10025,16 +10025,16 @@
         <v>0</v>
       </c>
       <c r="B7" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="15" t="s">
+      <c r="E7" s="16" t="s">
         <v>31</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="240">
@@ -10042,16 +10042,16 @@
         <v>2</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="E8" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="345">
@@ -10059,16 +10059,16 @@
         <v>3</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="D9" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="E9" s="19" t="s">
         <v>39</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -10115,180 +10115,180 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="24"/>
+        <v>57</v>
+      </c>
+      <c r="B1" s="23"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="23" t="s">
         <v>42</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="24" t="s">
         <v>44</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>49</v>
+        <v>46</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>93</v>
+        <v>56</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>52</v>
+        <v>49</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="23" t="s">
         <v>54</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>53</v>
+        <v>50</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>94</v>
+        <v>55</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>95</v>
+        <v>58</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="23" t="s">
         <v>62</v>
-      </c>
-      <c r="B12" s="24" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13" s="24" t="s">
-        <v>64</v>
+        <v>60</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" s="24" t="s">
-        <v>65</v>
+        <v>59</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="23" t="s">
         <v>66</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" s="24" t="s">
-        <v>96</v>
+        <v>67</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="23" t="s">
         <v>69</v>
-      </c>
-      <c r="B17" s="24" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>71</v>
-      </c>
-      <c r="B18" s="24" t="s">
-        <v>97</v>
+        <v>70</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>72</v>
-      </c>
-      <c r="B19" s="24" t="s">
-        <v>75</v>
+        <v>71</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>73</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>74</v>
-      </c>
-      <c r="B21" s="24" t="s">
-        <v>67</v>
+        <v>73</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="45">
-      <c r="A22" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="B22" s="24" t="s">
+      <c r="A22" s="22" t="s">
         <v>77</v>
       </c>
+      <c r="B22" s="23" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="B24" s="24"/>
+      <c r="B24" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10310,7 +10310,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B1">
         <v>39225</v>
@@ -10321,7 +10321,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2">
         <v>4308</v>
@@ -10332,7 +10332,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3">
         <v>-3542</v>
@@ -10343,7 +10343,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4">
         <f>B1*-0.05</f>
@@ -10356,7 +10356,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5">
         <v>-11000</v>
@@ -10367,7 +10367,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B6">
         <f>SUM(B1:B5)</f>
@@ -10384,7 +10384,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7">
         <f>B6/2</f>
@@ -10397,7 +10397,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B9">
         <v>3500</v>
@@ -10405,7 +10405,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B10">
         <v>2500</v>
@@ -10413,7 +10413,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B11">
         <v>6000</v>
@@ -10421,7 +10421,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B12">
         <v>6000</v>
@@ -10429,7 +10429,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B13">
         <v>2500</v>
@@ -10437,7 +10437,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B14">
         <v>1000</v>
@@ -10453,12 +10453,12 @@
         <v>21500</v>
       </c>
       <c r="D15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B16">
         <f>B6-B15</f>

</xml_diff>